<commit_message>
set demo template as default if secrets doesnt exist
</commit_message>
<xml_diff>
--- a/electron-react-app/src/DemoTemplate/template PO_demo.xlsx
+++ b/electron-react-app/src/DemoTemplate/template PO_demo.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quant\Desktop\POPRFiller_Windows\Template for 2.1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C000BBB-26AD-4DF5-ABDE-4BC32D8F360A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6129E015-A806-4049-88CC-5AE3B5D72CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8400" yWindow="2550" windowWidth="28980" windowHeight="16140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="8745" yWindow="2895" windowWidth="28980" windowHeight="16140" xr2:uid="{A483AB3D-0902-45D6-A276-0FFF3149B3B7}"/>
+    <workbookView xWindow="14745" yWindow="2970" windowWidth="33165" windowHeight="16140" xr2:uid="{A483AB3D-0902-45D6-A276-0FFF3149B3B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Purchase Requisition" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Project X</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -78,18 +77,6 @@
   </si>
   <si>
     <t>1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -311,7 +298,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -353,37 +340,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="dotted">
         <color auto="1"/>
       </left>
@@ -416,17 +372,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="dotted">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -517,17 +462,16 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -546,21 +490,25 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="40" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -569,12 +517,12 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -584,26 +532,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -885,13 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J54"/>
+  <dimension ref="B1:J51"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="1">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -909,41 +838,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="21" x14ac:dyDescent="0.3">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.3">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="31">
+        <v>18</v>
+      </c>
+      <c r="H4" s="32">
         <f>PO_Input!D3</f>
         <v>0</v>
       </c>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
     </row>
     <row r="5" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
@@ -969,26 +898,26 @@
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="25">
+        <v>42</v>
+      </c>
+      <c r="C9" s="26">
         <f>PO_Input!B3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="25"/>
+      <c r="D9" s="26"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="25">
+        <v>20</v>
+      </c>
+      <c r="C11" s="26">
         <f>PO_Input!C3</f>
         <v>0</v>
       </c>
-      <c r="D11" s="25"/>
+      <c r="D11" s="26"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
@@ -1005,7 +934,7 @@
       <c r="B15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="33">
         <f>PO_Input!I3</f>
         <v>0</v>
       </c>
@@ -1019,14 +948,14 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
@@ -1035,24 +964,24 @@
       <c r="B18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="25">
+      <c r="C18" s="26">
         <f>PO_Input!G3</f>
         <v>0</v>
       </c>
-      <c r="D18" s="25"/>
+      <c r="D18" s="26"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="24">
+        <v>19</v>
+      </c>
+      <c r="C20" s="26">
         <f>PO_Input!H3</f>
         <v>0</v>
       </c>
-      <c r="D20" s="25"/>
+      <c r="D20" s="26"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
@@ -1061,24 +990,24 @@
       <c r="B22" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="26">
+      <c r="C22" s="27">
         <f>PO_Input!J3</f>
         <v>0</v>
       </c>
-      <c r="D22" s="25"/>
+      <c r="D22" s="26"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="25">
+        <v>21</v>
+      </c>
+      <c r="C24" s="26">
         <f>PO_Input!F3</f>
         <v>0</v>
       </c>
-      <c r="D24" s="25"/>
+      <c r="D24" s="26"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
@@ -1087,120 +1016,90 @@
       <c r="B26" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7"/>
+      <c r="D26" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="27" t="s">
+      <c r="G26" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="29"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
-      <c r="J27" s="9"/>
+      <c r="J27" s="8"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="3"/>
-      <c r="D28" s="3" t="str">
+      <c r="D28" s="34" t="str">
         <f>IF(PO_Input!L3="","", PO_Input!L3)</f>
         <v/>
       </c>
-      <c r="E28" s="36" t="str">
+      <c r="E28" s="22" t="str">
         <f>IF(PO_Input!K3="","", G28-F28)</f>
         <v/>
       </c>
-      <c r="F28" s="36" t="str">
+      <c r="F28" s="22" t="str">
         <f>IF(PO_Input!K3="","", PO_Input!K3)</f>
         <v/>
       </c>
-      <c r="G28" s="37" t="str">
+      <c r="G28" s="23" t="str">
         <f>IF(PO_Input!K3="","", C22)</f>
         <v/>
       </c>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="39"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="4"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="39"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
+      <c r="C30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+      <c r="C31" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="39"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="39"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="B33" s="4"/>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
-      <c r="C34" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
-      <c r="C35" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="4"/>
-      <c r="C36" t="s">
-        <v>26</v>
+      <c r="B36" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
@@ -1210,82 +1109,71 @@
       <c r="B38" s="4"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="2"/>
+      <c r="E39" s="2"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
+      <c r="C40" s="20">
+        <f>PO_Input!Q3</f>
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="4"/>
-      <c r="C42" s="2"/>
-      <c r="E42" s="2"/>
+      <c r="B42" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" s="4"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
-      <c r="C43" s="23">
-        <f>PO_Input!Q3</f>
-        <v>0</v>
-      </c>
-      <c r="E43" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="I45" s="2"/>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="4"/>
+      <c r="E46" t="s">
+        <v>25</v>
+      </c>
+      <c r="I46" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="4"/>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B48" s="4"/>
-      <c r="C48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="I48" s="2"/>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="4"/>
-      <c r="E49" t="s">
-        <v>28</v>
-      </c>
-      <c r="I49" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C53" s="2"/>
-      <c r="E53" s="2"/>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E54" t="s">
-        <v>28</v>
+      <c r="B47" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C50" s="2"/>
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="12">
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="G26:J26"/>
@@ -1296,9 +1184,6 @@
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="G28:J28"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="G30:J30"/>
-    <mergeCell ref="G31:J31"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C22:D22"/>
   </mergeCells>
@@ -1311,11 +1196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3D1BCA0-37F2-4FF5-A9BD-76AA820C9F6E}">
   <dimension ref="A2:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="K3" sqref="J3:K3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1325,72 +1207,72 @@
   <sheetData>
     <row r="2" spans="1:17" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="E2" s="9"/>
+      <c r="F2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10" t="s">
+      <c r="I2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="J2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="K2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="M2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="N2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="O2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="P2" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="Q2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="O2" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="P2" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q2" s="13" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="22"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>